<commit_message>
und bild wurde ich abgeben
</commit_message>
<xml_diff>
--- a/Aufgabe9/Linear_Binary_Search.xlsx
+++ b/Aufgabe9/Linear_Binary_Search.xlsx
@@ -32,15 +32,6 @@
     <t>binäre Suche</t>
   </si>
   <si>
-    <t>Meine in ns</t>
-  </si>
-  <si>
-    <t>lin</t>
-  </si>
-  <si>
-    <t>bin</t>
-  </si>
-  <si>
     <t>Geschwindigkeit hangt von mehreren Faktoren ab:</t>
   </si>
   <si>
@@ -51,6 +42,15 @@
   </si>
   <si>
     <t>und z.B allgemeinem Alter vom PC</t>
+  </si>
+  <si>
+    <t>Anzahl der Elementen in ns</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>binary</t>
   </si>
 </sst>
 </file>
@@ -275,11 +275,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="242711968"/>
-        <c:axId val="242713536"/>
+        <c:axId val="330721872"/>
+        <c:axId val="330722264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242711968"/>
+        <c:axId val="330721872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,7 +308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242713536"/>
+        <c:crossAx val="330722264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -316,7 +316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242713536"/>
+        <c:axId val="330722264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="900000"/>
@@ -328,7 +328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242711968"/>
+        <c:crossAx val="330721872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -400,7 +400,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lin</c:v>
+                  <c:v>linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -482,7 +482,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>bin</c:v>
+                  <c:v>binary</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -565,11 +565,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="242712360"/>
-        <c:axId val="242713144"/>
+        <c:axId val="330725792"/>
+        <c:axId val="207496464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242712360"/>
+        <c:axId val="330725792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242713144"/>
+        <c:crossAx val="207496464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242713144"/>
+        <c:axId val="207496464"/>
         <c:scaling>
           <c:logBase val="9"/>
           <c:orientation val="minMax"/>
@@ -674,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242712360"/>
+        <c:crossAx val="330725792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1303,13 +1303,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -1332,16 +1332,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>42861</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>628649</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1652,15 +1652,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1674,13 +1677,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1723,10 +1726,10 @@
         <v>326369</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1749,7 +1752,7 @@
         <v>364571</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1772,7 +1775,7 @@
         <v>1569124</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neues. Habe dein messung gelost, deswegen wenn notig speicher noch dein excel irgendwo anders. Damit nicht uberschrieben wird
</commit_message>
<xml_diff>
--- a/Aufgabe9/Linear_Binary_Search.xlsx
+++ b/Aufgabe9/Linear_Binary_Search.xlsx
@@ -21,16 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>lineare Suche</t>
-  </si>
-  <si>
-    <t>binäre Suche</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Geschwindigkeit hangt von mehreren Faktoren ab:</t>
   </si>
@@ -41,9 +32,6 @@
     <t>Geschwindigkeit von Harddisk</t>
   </si>
   <si>
-    <t>und z.B allgemeinem Alter vom PC</t>
-  </si>
-  <si>
     <t>Anzahl der Elementen in ns</t>
   </si>
   <si>
@@ -51,6 +39,9 @@
   </si>
   <si>
     <t>binary</t>
+  </si>
+  <si>
+    <t>usw.</t>
   </si>
 </sst>
 </file>
@@ -143,248 +134,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lineare Suche</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1198723</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1231385</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1351771</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1462824</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>binäre Suche</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>959818</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>992480</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1049874</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1325640</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="330721872"/>
-        <c:axId val="330722264"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="330721872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>n Anzahl der  Elementen in der Liste</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330722264"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="330722264"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="900000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330721872"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="thousands"/>
-          <c:dispUnitsLbl>
-            <c:layout/>
-            <c:tx>
-              <c:rich>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:r>
-                    <a:rPr lang="en-US"/>
-                    <a:t>Mikrosekunden</a:t>
-                  </a:r>
-                </a:p>
-              </c:rich>
-            </c:tx>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
@@ -396,7 +145,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$G$1</c:f>
+              <c:f>Tabelle1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -431,7 +180,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$5</c:f>
+              <c:f>Tabelle1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -452,7 +201,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$5</c:f>
+              <c:f>Tabelle1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -478,7 +227,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$H$1</c:f>
+              <c:f>Tabelle1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -513,7 +262,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$5</c:f>
+              <c:f>Tabelle1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -534,7 +283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$2:$H$5</c:f>
+              <c:f>Tabelle1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -565,11 +314,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="330725792"/>
-        <c:axId val="207496464"/>
+        <c:axId val="326923432"/>
+        <c:axId val="326922256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="330725792"/>
+        <c:axId val="326923432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207496464"/>
+        <c:crossAx val="326922256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="207496464"/>
+        <c:axId val="326922256"/>
         <c:scaling>
           <c:logBase val="9"/>
           <c:orientation val="minMax"/>
@@ -674,7 +423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330725792"/>
+        <c:crossAx val="326923432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1302,43 +1051,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>600074</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>628649</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -1354,7 +1073,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1650,131 +1369,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10000</v>
       </c>
       <c r="B2" s="1">
-        <v>1198723</v>
+        <v>2197905</v>
       </c>
       <c r="C2" s="1">
-        <v>959818</v>
-      </c>
-      <c r="F2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2197905</v>
-      </c>
-      <c r="H2" s="1">
         <v>232991</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100000</v>
       </c>
       <c r="B3" s="1">
-        <v>1231385</v>
+        <v>8494865</v>
       </c>
       <c r="C3" s="1">
-        <v>992480</v>
-      </c>
-      <c r="F3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="1">
-        <v>8494865</v>
-      </c>
-      <c r="H3" s="1">
         <v>326369</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>4</v>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1000000</v>
       </c>
       <c r="B4" s="1">
-        <v>1351771</v>
+        <v>17028003</v>
       </c>
       <c r="C4" s="1">
-        <v>1049874</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>17028003</v>
-      </c>
-      <c r="H4" s="1">
         <v>364571</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>5</v>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10000000</v>
       </c>
       <c r="B5" s="1">
-        <v>1462824</v>
+        <v>123726759</v>
       </c>
       <c r="C5" s="1">
-        <v>1325640</v>
-      </c>
-      <c r="F5" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="G5" s="1">
-        <v>123726759</v>
-      </c>
-      <c r="H5" s="1">
         <v>1569124</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>